<commit_message>
correct manybugs output archive and chunks data
</commit_message>
<xml_diff>
--- a/5. ManyBugs_C_Metrics/ManyBugs_19_Complexity_Avg.xlsx
+++ b/5. ManyBugs_C_Metrics/ManyBugs_19_Complexity_Avg.xlsx
@@ -1059,9 +1059,6 @@
     <t>Avg-Buggy</t>
   </si>
   <si>
-    <t>Multi-Hunk &amp; Multi-Line</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -1149,12 +1146,6 @@
     <t>Avg-manual</t>
   </si>
   <si>
-    <t>Single-Hunk-Avg-manual</t>
-  </si>
-  <si>
-    <t>Multi-Hunk-Avg-manual</t>
-  </si>
-  <si>
     <t>Single-Line-Avg-manual</t>
   </si>
   <si>
@@ -1233,12 +1224,6 @@
     <t>Avg-auto</t>
   </si>
   <si>
-    <t>Single-Hunk-Avg-auto</t>
-  </si>
-  <si>
-    <t>Multi-Hunk-Avg-auto</t>
-  </si>
-  <si>
     <t>Single-Line-Avg-auto</t>
   </si>
   <si>
@@ -1255,6 +1240,21 @@
   </si>
   <si>
     <t>Avg-Machine Learning-auto</t>
+  </si>
+  <si>
+    <t>Multi-Chunk &amp; Multi-Line</t>
+  </si>
+  <si>
+    <t>Single-Chunk-Avg-manual</t>
+  </si>
+  <si>
+    <t>Single-Chunk-Avg-auto</t>
+  </si>
+  <si>
+    <t>Multi-Chunk-Avg-manual</t>
+  </si>
+  <si>
+    <t>Multi-Chunk-Avg-auto</t>
   </si>
 </sst>
 </file>
@@ -2401,8 +2401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X131"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K27" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43:X80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A80" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.35"/>
@@ -2530,12 +2530,12 @@
     <row r="22" spans="1:24" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="S22" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:24" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>20</v>
@@ -2589,22 +2589,22 @@
         <v>70</v>
       </c>
       <c r="S23" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="T23" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="T23" s="37" t="s">
+      <c r="U23" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="U23" s="37" t="s">
-        <v>109</v>
-      </c>
       <c r="V23" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="W23" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="W23" s="37" t="s">
+      <c r="X23" s="37" t="s">
         <v>112</v>
-      </c>
-      <c r="X23" s="37" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.35">
@@ -2661,7 +2661,7 @@
         <v>74</v>
       </c>
       <c r="R24" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A24))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A24))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A24))), "auto", "")))</f>
+        <f t="shared" ref="R24:R55" si="1">IF(NOT(ISERR(SEARCH("*-buggy",$A24))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A24))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A24))), "auto", "")))</f>
         <v>Buggy</v>
       </c>
       <c r="S24" s="15"/>
@@ -2715,7 +2715,7 @@
         <v>447.91</v>
       </c>
       <c r="O25" s="15" t="str">
-        <f t="shared" ref="O25:O36" si="1">LEFT($A25,FIND("-",$A25)-1)</f>
+        <f t="shared" ref="O25:O36" si="2">LEFT($A25,FIND("-",$A25)-1)</f>
         <v>angelix</v>
       </c>
       <c r="P25" s="15" t="s">
@@ -2725,7 +2725,7 @@
         <v>74</v>
       </c>
       <c r="R25" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A25))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A25))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A25))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S25" s="15"/>
@@ -2779,7 +2779,7 @@
         <v>513.53</v>
       </c>
       <c r="O26" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>angelix</v>
       </c>
       <c r="P26" s="15" t="s">
@@ -2789,7 +2789,7 @@
         <v>75</v>
       </c>
       <c r="R26" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A26))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A26))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A26))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S26" s="15"/>
@@ -2843,7 +2843,7 @@
         <v>82.83</v>
       </c>
       <c r="O27" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>angelix</v>
       </c>
       <c r="P27" s="15" t="s">
@@ -2853,7 +2853,7 @@
         <v>76</v>
       </c>
       <c r="R27" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A27))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A27))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A27))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S27" s="15"/>
@@ -2907,7 +2907,7 @@
         <v>61.5</v>
       </c>
       <c r="O28" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>angelix</v>
       </c>
       <c r="P28" s="15" t="s">
@@ -2917,7 +2917,7 @@
         <v>77</v>
       </c>
       <c r="R28" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A28))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A28))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A28))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S28" s="15"/>
@@ -2971,7 +2971,7 @@
         <v>115.31</v>
       </c>
       <c r="O29" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>angelix</v>
       </c>
       <c r="P29" s="15" t="s">
@@ -2981,7 +2981,7 @@
         <v>78</v>
       </c>
       <c r="R29" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A29))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A29))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A29))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S29" s="15"/>
@@ -3035,7 +3035,7 @@
         <v>41.27</v>
       </c>
       <c r="O30" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P30" s="15" t="s">
@@ -3045,7 +3045,7 @@
         <v>82</v>
       </c>
       <c r="R30" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A30))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A30))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A30))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S30" s="15"/>
@@ -3099,7 +3099,7 @@
         <v>513.53</v>
       </c>
       <c r="O31" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P31" s="15" t="s">
@@ -3109,7 +3109,7 @@
         <v>75</v>
       </c>
       <c r="R31" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A31))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A31))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A31))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S31" s="15"/>
@@ -3163,7 +3163,7 @@
         <v>61.5</v>
       </c>
       <c r="O32" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P32" s="15" t="s">
@@ -3173,7 +3173,7 @@
         <v>77</v>
       </c>
       <c r="R32" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A32))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A32))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A32))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S32" s="15"/>
@@ -3227,7 +3227,7 @@
         <v>61.5</v>
       </c>
       <c r="O33" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P33" s="15" t="s">
@@ -3237,7 +3237,7 @@
         <v>77</v>
       </c>
       <c r="R33" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A33))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A33))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A33))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S33" s="15"/>
@@ -3291,7 +3291,7 @@
         <v>52.78</v>
       </c>
       <c r="O34" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P34" s="15" t="s">
@@ -3301,7 +3301,7 @@
         <v>79</v>
       </c>
       <c r="R34" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A34))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A34))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A34))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S34" s="15"/>
@@ -3355,7 +3355,7 @@
         <v>15.67</v>
       </c>
       <c r="O35" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P35" s="15" t="s">
@@ -3365,7 +3365,7 @@
         <v>80</v>
       </c>
       <c r="R35" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A35))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A35))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A35))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S35" s="15"/>
@@ -3419,7 +3419,7 @@
         <v>4.93</v>
       </c>
       <c r="O36" s="15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>prophet</v>
       </c>
       <c r="P36" s="15" t="s">
@@ -3429,7 +3429,7 @@
         <v>83</v>
       </c>
       <c r="R36" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A36))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A36))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A36))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S36" s="15"/>
@@ -3483,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="O37" s="15" t="str">
-        <f t="shared" ref="O37:O48" si="2">LEFT($A37,FIND("-",$A37)-1)</f>
+        <f t="shared" ref="O37:O48" si="3">LEFT($A37,FIND("-",$A37)-1)</f>
         <v>prophet</v>
       </c>
       <c r="P37" s="15" t="s">
@@ -3493,7 +3493,7 @@
         <v>81</v>
       </c>
       <c r="R37" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A37))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A37))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A37))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S37" s="15"/>
@@ -3547,7 +3547,7 @@
         <v>50.93</v>
       </c>
       <c r="O38" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>prophet</v>
       </c>
       <c r="P38" s="15" t="s">
@@ -3557,7 +3557,7 @@
         <v>84</v>
       </c>
       <c r="R38" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A38))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A38))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A38))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S38" s="15"/>
@@ -3611,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="O39" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>prophet</v>
       </c>
       <c r="P39" s="15" t="s">
@@ -3621,7 +3621,7 @@
         <v>85</v>
       </c>
       <c r="R39" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A39))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A39))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A39))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S39" s="15"/>
@@ -3675,7 +3675,7 @@
         <v>6.69</v>
       </c>
       <c r="O40" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>prophet</v>
       </c>
       <c r="P40" s="15" t="s">
@@ -3685,7 +3685,7 @@
         <v>86</v>
       </c>
       <c r="R40" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A40))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A40))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A40))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S40" s="15"/>
@@ -3739,7 +3739,7 @@
         <v>50.93</v>
       </c>
       <c r="O41" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>prophet</v>
       </c>
       <c r="P41" s="15" t="s">
@@ -3749,7 +3749,7 @@
         <v>87</v>
       </c>
       <c r="R41" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A41))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A41))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A41))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S41" s="15"/>
@@ -3803,7 +3803,7 @@
         <v>23.37</v>
       </c>
       <c r="O42" s="23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>prophet</v>
       </c>
       <c r="P42" s="23" t="s">
@@ -3813,7 +3813,7 @@
         <v>88</v>
       </c>
       <c r="R42" s="23" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A42))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A42))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A42))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>Buggy</v>
       </c>
       <c r="S42" s="23"/>
@@ -3825,7 +3825,7 @@
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B43" s="19">
         <v>9.57</v>
@@ -3867,7 +3867,7 @@
         <v>447.91</v>
       </c>
       <c r="O43" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>angelix</v>
       </c>
       <c r="P43" s="20" t="s">
@@ -3877,31 +3877,31 @@
         <v>74</v>
       </c>
       <c r="R43" s="20" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A43))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A43))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A43))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S43" s="20">
+        <v>2</v>
+      </c>
+      <c r="T43" s="20">
+        <v>0</v>
+      </c>
+      <c r="U43" s="20">
         <v>1</v>
       </c>
-      <c r="T43" s="20">
-        <v>0</v>
-      </c>
-      <c r="U43" s="20">
-        <v>0</v>
-      </c>
       <c r="V43" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W43" s="20">
         <v>0</v>
       </c>
       <c r="X43" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B44" s="9">
         <v>9.57</v>
@@ -3943,7 +3943,7 @@
         <v>447.91</v>
       </c>
       <c r="O44" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>angelix</v>
       </c>
       <c r="P44" s="15" t="s">
@@ -3953,31 +3953,31 @@
         <v>74</v>
       </c>
       <c r="R44" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A44))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A44))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A44))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S44" s="15">
+        <v>2</v>
+      </c>
+      <c r="T44" s="15">
+        <v>0</v>
+      </c>
+      <c r="U44" s="15">
         <v>1</v>
       </c>
-      <c r="T44" s="15">
-        <v>0</v>
-      </c>
-      <c r="U44" s="15">
-        <v>0</v>
-      </c>
       <c r="V44" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W44" s="15">
         <v>0</v>
       </c>
       <c r="X44" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="9">
         <v>5.42</v>
@@ -4019,7 +4019,7 @@
         <v>513.53</v>
       </c>
       <c r="O45" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>angelix</v>
       </c>
       <c r="P45" s="15" t="s">
@@ -4029,11 +4029,11 @@
         <v>75</v>
       </c>
       <c r="R45" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A45))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A45))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A45))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S45" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T45" s="15">
         <v>0</v>
@@ -4042,18 +4042,18 @@
         <v>0</v>
       </c>
       <c r="V45" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W45" s="15">
         <v>0</v>
       </c>
       <c r="X45" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B46" s="7">
         <v>5.26</v>
@@ -4095,7 +4095,7 @@
         <v>82.83</v>
       </c>
       <c r="O46" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>angelix</v>
       </c>
       <c r="P46" s="15" t="s">
@@ -4105,7 +4105,7 @@
         <v>76</v>
       </c>
       <c r="R46" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A46))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A46))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A46))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S46" s="15">
@@ -4115,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="U46" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V46" s="15">
         <v>1</v>
@@ -4124,12 +4124,12 @@
         <v>0</v>
       </c>
       <c r="X46" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B47" s="9">
         <v>4.2699999999999996</v>
@@ -4171,7 +4171,7 @@
         <v>61.2</v>
       </c>
       <c r="O47" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>angelix</v>
       </c>
       <c r="P47" s="15" t="s">
@@ -4181,31 +4181,31 @@
         <v>77</v>
       </c>
       <c r="R47" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A47))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A47))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A47))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S47" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T47" s="15">
         <v>0</v>
       </c>
       <c r="U47" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V47" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W47" s="15">
         <v>0</v>
       </c>
       <c r="X47" s="15">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" s="7">
         <v>7.75</v>
@@ -4247,7 +4247,7 @@
         <v>115.31</v>
       </c>
       <c r="O48" s="15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>angelix</v>
       </c>
       <c r="P48" s="15" t="s">
@@ -4257,7 +4257,7 @@
         <v>78</v>
       </c>
       <c r="R48" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A48))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A48))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A48))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S48" s="15">
@@ -4281,7 +4281,7 @@
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" s="9">
         <v>2.5</v>
@@ -4323,7 +4323,7 @@
         <v>41.27</v>
       </c>
       <c r="O49" s="15" t="str">
-        <f t="shared" ref="O49:O67" si="3">LEFT($A49,FIND("-",$A49)-1)</f>
+        <f t="shared" ref="O49:O67" si="4">LEFT($A49,FIND("-",$A49)-1)</f>
         <v>prophet</v>
       </c>
       <c r="P49" s="15" t="s">
@@ -4333,14 +4333,14 @@
         <v>82</v>
       </c>
       <c r="R49" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A49))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A49))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A49))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S49" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U49" s="15">
         <v>0</v>
@@ -4352,12 +4352,12 @@
         <v>0</v>
       </c>
       <c r="X49" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" s="7">
         <v>5.42</v>
@@ -4399,7 +4399,7 @@
         <v>513.53</v>
       </c>
       <c r="O50" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P50" s="15" t="s">
@@ -4409,11 +4409,11 @@
         <v>75</v>
       </c>
       <c r="R50" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A50))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A50))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A50))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S50" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50" s="15">
         <v>0</v>
@@ -4422,18 +4422,18 @@
         <v>0</v>
       </c>
       <c r="V50" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W50" s="15">
         <v>0</v>
       </c>
       <c r="X50" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" s="7">
         <v>4.2699999999999996</v>
@@ -4475,7 +4475,7 @@
         <v>61.2</v>
       </c>
       <c r="O51" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P51" s="15" t="s">
@@ -4485,31 +4485,31 @@
         <v>77</v>
       </c>
       <c r="R51" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A51))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A51))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A51))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S51" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T51" s="15">
         <v>0</v>
       </c>
       <c r="U51" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V51" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W51" s="15">
         <v>0</v>
       </c>
       <c r="X51" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" s="9">
         <v>4.2699999999999996</v>
@@ -4551,7 +4551,7 @@
         <v>61.2</v>
       </c>
       <c r="O52" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P52" s="15" t="s">
@@ -4561,31 +4561,31 @@
         <v>77</v>
       </c>
       <c r="R52" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A52))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A52))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A52))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S52" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T52" s="15">
         <v>0</v>
       </c>
       <c r="U52" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V52" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W52" s="15">
         <v>0</v>
       </c>
       <c r="X52" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="9">
         <v>2.33</v>
@@ -4627,7 +4627,7 @@
         <v>53.89</v>
       </c>
       <c r="O53" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P53" s="15" t="s">
@@ -4637,14 +4637,14 @@
         <v>79</v>
       </c>
       <c r="R53" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A53))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A53))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A53))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S53" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T53" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53" s="15">
         <v>0</v>
@@ -4656,12 +4656,12 @@
         <v>0</v>
       </c>
       <c r="X53" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" s="7">
         <v>5.25</v>
@@ -4703,7 +4703,7 @@
         <v>15.67</v>
       </c>
       <c r="O54" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P54" s="15" t="s">
@@ -4713,11 +4713,11 @@
         <v>80</v>
       </c>
       <c r="R54" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A54))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A54))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A54))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S54" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T54" s="15">
         <v>0</v>
@@ -4726,18 +4726,18 @@
         <v>0</v>
       </c>
       <c r="V54" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W54" s="15">
         <v>0</v>
       </c>
       <c r="X54" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A55" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" s="9">
         <v>2.67</v>
@@ -4779,7 +4779,7 @@
         <v>4.93</v>
       </c>
       <c r="O55" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P55" s="15" t="s">
@@ -4789,14 +4789,14 @@
         <v>83</v>
       </c>
       <c r="R55" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A55))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A55))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A55))), "auto", "")))</f>
+        <f t="shared" si="1"/>
         <v>manual</v>
       </c>
       <c r="S55" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T55" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U55" s="15">
         <v>0</v>
@@ -4808,12 +4808,12 @@
         <v>0</v>
       </c>
       <c r="X55" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B56" s="7">
         <v>1</v>
@@ -4855,7 +4855,7 @@
         <v>0</v>
       </c>
       <c r="O56" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P56" s="15" t="s">
@@ -4865,31 +4865,31 @@
         <v>81</v>
       </c>
       <c r="R56" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A56))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A56))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A56))), "auto", "")))</f>
+        <f t="shared" ref="R56:R80" si="5">IF(NOT(ISERR(SEARCH("*-buggy",$A56))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A56))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A56))), "auto", "")))</f>
         <v>manual</v>
       </c>
       <c r="S56" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T56" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U56" s="15">
         <v>0</v>
       </c>
       <c r="V56" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W56" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X56" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A57" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B57" s="9">
         <v>5</v>
@@ -4931,7 +4931,7 @@
         <v>50.93</v>
       </c>
       <c r="O57" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P57" s="15" t="s">
@@ -4941,11 +4941,11 @@
         <v>84</v>
       </c>
       <c r="R57" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A57))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A57))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A57))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>manual</v>
       </c>
       <c r="S57" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T57" s="15">
         <v>0</v>
@@ -4954,18 +4954,18 @@
         <v>0</v>
       </c>
       <c r="V57" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W57" s="15">
         <v>0</v>
       </c>
       <c r="X57" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B58" s="7">
         <v>1</v>
@@ -5007,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="O58" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P58" s="15" t="s">
@@ -5017,11 +5017,11 @@
         <v>85</v>
       </c>
       <c r="R58" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A58))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A58))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A58))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>manual</v>
       </c>
       <c r="S58" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T58" s="15">
         <v>0</v>
@@ -5030,18 +5030,18 @@
         <v>0</v>
       </c>
       <c r="V58" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W58" s="15">
         <v>0</v>
       </c>
       <c r="X58" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="9">
         <v>2.0699999999999998</v>
@@ -5083,7 +5083,7 @@
         <v>6.69</v>
       </c>
       <c r="O59" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P59" s="15" t="s">
@@ -5093,11 +5093,11 @@
         <v>86</v>
       </c>
       <c r="R59" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A59))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A59))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A59))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>manual</v>
       </c>
       <c r="S59" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T59" s="15">
         <v>0</v>
@@ -5106,18 +5106,18 @@
         <v>0</v>
       </c>
       <c r="V59" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W59" s="15">
         <v>0</v>
       </c>
       <c r="X59" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B60" s="7">
         <v>5</v>
@@ -5159,7 +5159,7 @@
         <v>50.93</v>
       </c>
       <c r="O60" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P60" s="15" t="s">
@@ -5169,11 +5169,11 @@
         <v>87</v>
       </c>
       <c r="R60" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A60))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A60))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A60))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>manual</v>
       </c>
       <c r="S60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T60" s="15">
         <v>0</v>
@@ -5182,18 +5182,18 @@
         <v>0</v>
       </c>
       <c r="V60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W60" s="15">
         <v>0</v>
       </c>
       <c r="X60" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="22">
         <v>2.82</v>
@@ -5235,7 +5235,7 @@
         <v>23.8</v>
       </c>
       <c r="O61" s="23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>prophet</v>
       </c>
       <c r="P61" s="23" t="s">
@@ -5245,31 +5245,31 @@
         <v>88</v>
       </c>
       <c r="R61" s="23" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A61))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A61))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A61))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>manual</v>
       </c>
       <c r="S61" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T61" s="23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U61" s="23">
         <v>0</v>
       </c>
       <c r="V61" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W61" s="23">
         <v>0</v>
       </c>
       <c r="X61" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A62" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B62" s="19">
         <v>9.57</v>
@@ -5311,7 +5311,7 @@
         <v>491.18</v>
       </c>
       <c r="O62" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>angelix</v>
       </c>
       <c r="P62" s="20" t="s">
@@ -5321,31 +5321,31 @@
         <v>74</v>
       </c>
       <c r="R62" s="20" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A62))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A62))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A62))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S62" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T62" s="20">
         <v>0</v>
       </c>
       <c r="U62" s="20">
+        <v>0</v>
+      </c>
+      <c r="V62" s="20">
         <v>1</v>
       </c>
-      <c r="V62" s="20">
-        <v>2</v>
-      </c>
       <c r="W62" s="20">
         <v>0</v>
       </c>
       <c r="X62" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A63" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B63" s="9">
         <v>9.7100000000000009</v>
@@ -5387,7 +5387,7 @@
         <v>461.11</v>
       </c>
       <c r="O63" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>angelix</v>
       </c>
       <c r="P63" s="15" t="s">
@@ -5397,31 +5397,31 @@
         <v>74</v>
       </c>
       <c r="R63" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A63))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A63))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A63))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S63" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T63" s="15">
         <v>0</v>
       </c>
       <c r="U63" s="15">
+        <v>0</v>
+      </c>
+      <c r="V63" s="15">
         <v>1</v>
       </c>
-      <c r="V63" s="15">
-        <v>2</v>
-      </c>
       <c r="W63" s="15">
         <v>0</v>
       </c>
       <c r="X63" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B64" s="7">
         <v>5.42</v>
@@ -5463,7 +5463,7 @@
         <v>513.53</v>
       </c>
       <c r="O64" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>angelix</v>
       </c>
       <c r="P64" s="15" t="s">
@@ -5473,11 +5473,11 @@
         <v>75</v>
       </c>
       <c r="R64" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A64))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A64))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A64))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S64" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="T64" s="15">
         <v>0</v>
@@ -5486,18 +5486,18 @@
         <v>0</v>
       </c>
       <c r="V64" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W64" s="15">
         <v>0</v>
       </c>
       <c r="X64" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A65" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B65" s="9">
         <v>5.26</v>
@@ -5539,7 +5539,7 @@
         <v>82.83</v>
       </c>
       <c r="O65" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>angelix</v>
       </c>
       <c r="P65" s="15" t="s">
@@ -5549,7 +5549,7 @@
         <v>76</v>
       </c>
       <c r="R65" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A65))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A65))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A65))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S65" s="15">
@@ -5559,7 +5559,7 @@
         <v>0</v>
       </c>
       <c r="U65" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V65" s="15">
         <v>1</v>
@@ -5568,12 +5568,12 @@
         <v>0</v>
       </c>
       <c r="X65" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B66" s="7">
         <v>4.2699999999999996</v>
@@ -5615,7 +5615,7 @@
         <v>61.5</v>
       </c>
       <c r="O66" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>angelix</v>
       </c>
       <c r="P66" s="15" t="s">
@@ -5625,31 +5625,31 @@
         <v>77</v>
       </c>
       <c r="R66" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A66))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A66))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A66))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S66" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T66" s="15">
         <v>0</v>
       </c>
       <c r="U66" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V66" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W66" s="15">
         <v>0</v>
       </c>
       <c r="X66" s="15">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A67" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B67" s="9">
         <v>7.75</v>
@@ -5691,7 +5691,7 @@
         <v>115.31</v>
       </c>
       <c r="O67" s="15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>angelix</v>
       </c>
       <c r="P67" s="15" t="s">
@@ -5701,7 +5701,7 @@
         <v>78</v>
       </c>
       <c r="R67" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A67))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A67))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A67))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S67" s="15">
@@ -5725,7 +5725,7 @@
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B68" s="7">
         <v>2.5</v>
@@ -5767,7 +5767,7 @@
         <v>41.27</v>
       </c>
       <c r="O68" s="15" t="str">
-        <f t="shared" ref="O68:O80" si="4">LEFT($A68,FIND("-",$A68)-1)</f>
+        <f t="shared" ref="O68:O80" si="6">LEFT($A68,FIND("-",$A68)-1)</f>
         <v>prophet</v>
       </c>
       <c r="P68" s="15" t="s">
@@ -5777,14 +5777,14 @@
         <v>82</v>
       </c>
       <c r="R68" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A68))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A68))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A68))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S68" s="15">
         <v>1</v>
       </c>
       <c r="T68" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U68" s="15">
         <v>0</v>
@@ -5796,12 +5796,12 @@
         <v>0</v>
       </c>
       <c r="X68" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A69" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B69" s="9">
         <v>5.42</v>
@@ -5843,7 +5843,7 @@
         <v>514.01</v>
       </c>
       <c r="O69" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P69" s="15" t="s">
@@ -5853,31 +5853,31 @@
         <v>75</v>
       </c>
       <c r="R69" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A69))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A69))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A69))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S69" s="15">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="T69" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U69" s="15">
         <v>0</v>
       </c>
       <c r="V69" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W69" s="15">
         <v>0</v>
       </c>
       <c r="X69" s="15">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B70" s="7">
         <v>4.2699999999999996</v>
@@ -5919,7 +5919,7 @@
         <v>61.5</v>
       </c>
       <c r="O70" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P70" s="15" t="s">
@@ -5929,23 +5929,23 @@
         <v>77</v>
       </c>
       <c r="R70" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A70))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A70))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A70))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S70" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T70" s="15">
         <v>0</v>
       </c>
       <c r="U70" s="15">
+        <v>2</v>
+      </c>
+      <c r="V70" s="15">
         <v>5</v>
       </c>
-      <c r="V70" s="15">
-        <v>2</v>
-      </c>
       <c r="W70" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X70" s="15">
         <v>7</v>
@@ -5953,7 +5953,7 @@
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A71" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B71" s="9">
         <v>4.29</v>
@@ -5995,7 +5995,7 @@
         <v>61.66</v>
       </c>
       <c r="O71" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P71" s="15" t="s">
@@ -6005,31 +6005,31 @@
         <v>77</v>
       </c>
       <c r="R71" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A71))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A71))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A71))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S71" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T71" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U71" s="15">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V71" s="15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W71" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X71" s="15">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B72" s="7">
         <v>2.33</v>
@@ -6071,7 +6071,7 @@
         <v>55.61</v>
       </c>
       <c r="O72" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P72" s="15" t="s">
@@ -6081,31 +6081,31 @@
         <v>79</v>
       </c>
       <c r="R72" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A72))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A72))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A72))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S72" s="15">
+        <v>2</v>
+      </c>
+      <c r="T72" s="15">
+        <v>2</v>
+      </c>
+      <c r="U72" s="15">
+        <v>0</v>
+      </c>
+      <c r="V72" s="15">
         <v>1</v>
       </c>
-      <c r="T72" s="15">
-        <v>1</v>
-      </c>
-      <c r="U72" s="15">
-        <v>0</v>
-      </c>
-      <c r="V72" s="15">
-        <v>0</v>
-      </c>
       <c r="W72" s="15">
         <v>0</v>
       </c>
       <c r="X72" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A73" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B73" s="9">
         <v>5.25</v>
@@ -6147,7 +6147,7 @@
         <v>15.67</v>
       </c>
       <c r="O73" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P73" s="15" t="s">
@@ -6157,31 +6157,31 @@
         <v>80</v>
       </c>
       <c r="R73" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A73))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A73))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A73))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S73" s="15">
         <v>1</v>
       </c>
       <c r="T73" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U73" s="15">
         <v>0</v>
       </c>
       <c r="V73" s="15">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="W73" s="15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X73" s="15">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B74" s="7">
         <v>2.67</v>
@@ -6223,7 +6223,7 @@
         <v>4.93</v>
       </c>
       <c r="O74" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P74" s="15" t="s">
@@ -6233,14 +6233,14 @@
         <v>83</v>
       </c>
       <c r="R74" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A74))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A74))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A74))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S74" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T74" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U74" s="15">
         <v>0</v>
@@ -6252,12 +6252,12 @@
         <v>0</v>
       </c>
       <c r="X74" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A75" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B75" s="9">
         <v>1</v>
@@ -6299,7 +6299,7 @@
         <v>0</v>
       </c>
       <c r="O75" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P75" s="15" t="s">
@@ -6309,14 +6309,14 @@
         <v>81</v>
       </c>
       <c r="R75" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A75))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A75))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A75))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S75" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T75" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="U75" s="15">
         <v>0</v>
@@ -6325,15 +6325,15 @@
         <v>1</v>
       </c>
       <c r="W75" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X75" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B76" s="7">
         <v>5.14</v>
@@ -6375,7 +6375,7 @@
         <v>79.040000000000006</v>
       </c>
       <c r="O76" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P76" s="15" t="s">
@@ -6385,31 +6385,31 @@
         <v>84</v>
       </c>
       <c r="R76" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A76))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A76))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A76))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S76" s="15">
+        <v>2</v>
+      </c>
+      <c r="T76" s="15">
+        <v>3</v>
+      </c>
+      <c r="U76" s="15">
+        <v>0</v>
+      </c>
+      <c r="V76" s="15">
         <v>1</v>
       </c>
-      <c r="T76" s="15">
-        <v>0</v>
-      </c>
-      <c r="U76" s="15">
-        <v>0</v>
-      </c>
-      <c r="V76" s="15">
-        <v>2</v>
-      </c>
       <c r="W76" s="15">
         <v>0</v>
       </c>
       <c r="X76" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A77" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B77" s="9">
         <v>1</v>
@@ -6451,7 +6451,7 @@
         <v>0</v>
       </c>
       <c r="O77" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P77" s="15" t="s">
@@ -6461,14 +6461,14 @@
         <v>85</v>
       </c>
       <c r="R77" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A77))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A77))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A77))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S77" s="15">
         <v>1</v>
       </c>
       <c r="T77" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U77" s="15">
         <v>0</v>
@@ -6480,12 +6480,12 @@
         <v>0</v>
       </c>
       <c r="X77" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B78" s="7">
         <v>2.0699999999999998</v>
@@ -6527,7 +6527,7 @@
         <v>6.69</v>
       </c>
       <c r="O78" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P78" s="15" t="s">
@@ -6537,20 +6537,20 @@
         <v>86</v>
       </c>
       <c r="R78" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A78))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A78))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A78))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S78" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T78" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U78" s="15">
         <v>0</v>
       </c>
       <c r="V78" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W78" s="15">
         <v>0</v>
@@ -6561,7 +6561,7 @@
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A79" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B79" s="9">
         <v>5.14</v>
@@ -6603,7 +6603,7 @@
         <v>79.040000000000006</v>
       </c>
       <c r="O79" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P79" s="15" t="s">
@@ -6613,14 +6613,14 @@
         <v>87</v>
       </c>
       <c r="R79" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A79))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A79))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A79))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S79" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T79" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U79" s="15">
         <v>0</v>
@@ -6632,12 +6632,12 @@
         <v>0</v>
       </c>
       <c r="X79" s="15">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B80" s="7">
         <v>2.82</v>
@@ -6679,7 +6679,7 @@
         <v>23.44</v>
       </c>
       <c r="O80" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>prophet</v>
       </c>
       <c r="P80" s="15" t="s">
@@ -6689,11 +6689,11 @@
         <v>88</v>
       </c>
       <c r="R80" s="15" t="str">
-        <f>IF(NOT(ISERR(SEARCH("*-buggy",$A80))), "Buggy", IF(NOT(ISERR(SEARCH("*-manual",$A80))), "manual", IF(NOT(ISERR(SEARCH("*-auto",$A80))), "auto", "")))</f>
+        <f t="shared" si="5"/>
         <v>auto</v>
       </c>
       <c r="S80" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T80" s="15">
         <v>3</v>
@@ -6702,18 +6702,18 @@
         <v>0</v>
       </c>
       <c r="V80" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W80" s="15">
         <v>0</v>
       </c>
       <c r="X80" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:24" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>20</v>
@@ -6767,22 +6767,22 @@
         <v>70</v>
       </c>
       <c r="S81" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="T81" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="T81" s="37" t="s">
+      <c r="U81" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="U81" s="37" t="s">
-        <v>109</v>
-      </c>
       <c r="V81" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="W81" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="W81" s="37" t="s">
+      <c r="X81" s="37" t="s">
         <v>112</v>
-      </c>
-      <c r="X81" s="37" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:24" ht="15" x14ac:dyDescent="0.35">
@@ -6790,55 +6790,55 @@
         <v>64</v>
       </c>
       <c r="B82" s="16">
-        <f t="shared" ref="B82:N82" si="5">SUM(B24:B80)</f>
+        <f t="shared" ref="B82:N82" si="7">SUM(B24:B80)</f>
         <v>256.36999999999995</v>
       </c>
       <c r="C82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4542.7700000000004</v>
       </c>
       <c r="D82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>525.04000000000019</v>
       </c>
       <c r="E82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>983.8299999999997</v>
       </c>
       <c r="F82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>293.69</v>
       </c>
       <c r="G82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1114.8300000000002</v>
       </c>
       <c r="H82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2098.65</v>
       </c>
       <c r="I82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>818.66999999999973</v>
       </c>
       <c r="J82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10427.679999999998</v>
       </c>
       <c r="K82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>196.24999999999997</v>
       </c>
       <c r="L82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>17.110000000000003</v>
       </c>
       <c r="M82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10560.149999999998</v>
       </c>
       <c r="N82" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7773.14</v>
       </c>
       <c r="O82"/>
@@ -6851,55 +6851,55 @@
         <v>65</v>
       </c>
       <c r="B83" s="17">
-        <f t="shared" ref="B83:N83" si="6">AVERAGE(B24:B80)</f>
+        <f t="shared" ref="B83:N83" si="8">AVERAGE(B24:B80)</f>
         <v>4.4977192982456131</v>
       </c>
       <c r="C83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>79.697719298245616</v>
       </c>
       <c r="D83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.2112280701754425</v>
       </c>
       <c r="E83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>17.260175438596487</v>
       </c>
       <c r="F83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.1524561403508775</v>
       </c>
       <c r="G83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.55842105263158</v>
       </c>
       <c r="H83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>36.818421052631578</v>
       </c>
       <c r="I83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>14.362631578947363</v>
       </c>
       <c r="J83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>182.94175438596488</v>
       </c>
       <c r="K83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.4429824561403506</v>
       </c>
       <c r="L83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.30017543859649126</v>
       </c>
       <c r="M83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>391.11666666666656</v>
       </c>
       <c r="N83" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>136.37087719298245</v>
       </c>
       <c r="O83"/>
@@ -6912,55 +6912,55 @@
         <v>66</v>
       </c>
       <c r="B84" s="16">
-        <f t="shared" ref="B84:N84" si="7">MIN(B24:B80)</f>
+        <f t="shared" ref="B84:N84" si="9">MIN(B24:B80)</f>
         <v>1</v>
       </c>
       <c r="C84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>69.06</v>
       </c>
       <c r="D84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="K84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N84" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O84"/>
@@ -6973,55 +6973,55 @@
         <v>67</v>
       </c>
       <c r="B85" s="17">
-        <f t="shared" ref="B85:N85" si="8">MAX(B24:B80)</f>
+        <f t="shared" ref="B85:N85" si="10">MAX(B24:B80)</f>
         <v>9.7100000000000009</v>
       </c>
       <c r="C85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="D85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17.03</v>
       </c>
       <c r="E85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>39.15</v>
       </c>
       <c r="F85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="G85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>39.72</v>
       </c>
       <c r="H85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78.87</v>
       </c>
       <c r="I85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24.44</v>
       </c>
       <c r="J85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>437.17</v>
       </c>
       <c r="K85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6.86</v>
       </c>
       <c r="L85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.64</v>
       </c>
       <c r="M85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>970.07</v>
       </c>
       <c r="N85" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>514.01</v>
       </c>
       <c r="O85"/>
@@ -7034,55 +7034,55 @@
         <v>68</v>
       </c>
       <c r="B86" s="16">
-        <f t="shared" ref="B86:N86" si="9">_xlfn.STDEV.S(B24:B80)</f>
+        <f t="shared" ref="B86:N86" si="11">_xlfn.STDEV.S(B24:B80)</f>
         <v>2.4485513337655851</v>
       </c>
       <c r="C86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>8.9086152157703733</v>
       </c>
       <c r="D86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4.9691455395755595</v>
       </c>
       <c r="E86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>11.104092953763255</v>
       </c>
       <c r="F86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.4703074423336693</v>
       </c>
       <c r="G86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>12.539920794559848</v>
       </c>
       <c r="H86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>23.320728807334952</v>
       </c>
       <c r="I86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7.2787846135964092</v>
       </c>
       <c r="J86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>139.13314064391196</v>
       </c>
       <c r="K86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>2.0773652310699133</v>
       </c>
       <c r="L86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.16289228724254473</v>
       </c>
       <c r="M86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>370.76279950933605</v>
       </c>
       <c r="N86" s="16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>184.82155660722259</v>
       </c>
       <c r="O86"/>
@@ -7095,55 +7095,55 @@
         <v>69</v>
       </c>
       <c r="B87" s="17">
-        <f t="shared" ref="B87:N87" si="10">_xlfn.VAR.S(B24:B80)</f>
+        <f t="shared" ref="B87:N87" si="12">_xlfn.VAR.S(B24:B80)</f>
         <v>5.9954036340852257</v>
       </c>
       <c r="C87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>79.363425062655423</v>
       </c>
       <c r="D87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>24.692407393483677</v>
       </c>
       <c r="E87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>123.30088032581476</v>
       </c>
       <c r="F87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6.1024188596491138</v>
       </c>
       <c r="G87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>157.24961353383449</v>
       </c>
       <c r="H87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>543.85639210526222</v>
       </c>
       <c r="I87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>52.980705451127832</v>
       </c>
       <c r="J87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>19358.030825438582</v>
       </c>
       <c r="K87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.3154463032581543</v>
       </c>
       <c r="L87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.6533897243107698E-2</v>
       </c>
       <c r="M87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>137465.05350000013</v>
       </c>
       <c r="N87" s="17">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>34159.007786716786</v>
       </c>
       <c r="O87"/>
@@ -7172,7 +7172,7 @@
     </row>
     <row r="92" spans="1:24" ht="28.8" x14ac:dyDescent="0.35">
       <c r="B92" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C92" s="13" t="s">
         <v>92</v>
@@ -7219,169 +7219,169 @@
         <v>103</v>
       </c>
       <c r="C93" s="29">
-        <f t="shared" ref="C93:O93" si="11">AVERAGEIF($R$24:$R$80, "Buggy", B$24:B$80)</f>
+        <f t="shared" ref="C93:O93" si="13">AVERAGEIF($R$24:$R$80, "Buggy", B$24:B$80)</f>
         <v>4.4763157894736842</v>
       </c>
       <c r="D93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>79.945263157894743</v>
       </c>
       <c r="E93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9.165789473684212</v>
       </c>
       <c r="F93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>17.146315789473686</v>
       </c>
       <c r="G93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.0778947368421052</v>
       </c>
       <c r="H93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>19.382105263157897</v>
       </c>
       <c r="I93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>36.528947368421044</v>
       </c>
       <c r="J93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>14.242105263157892</v>
       </c>
       <c r="K93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>181.21631578947373</v>
       </c>
       <c r="L93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.4005263157894738</v>
       </c>
       <c r="M93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.30789473684210522</v>
       </c>
       <c r="N93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>443.81299999999999</v>
       </c>
       <c r="O93" s="29">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>134.32052631578946</v>
       </c>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B94" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", B$24:B$80)</f>
+        <f t="shared" ref="C94:O94" si="14">AVERAGEIF($R$24:$R$80, "manual", B$24:B$80)</f>
         <v>4.4968421052631573</v>
       </c>
       <c r="D94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", C$24:C$80)</f>
+        <f t="shared" si="14"/>
         <v>79.604736842105268</v>
       </c>
       <c r="E94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", D$24:D$80)</f>
+        <f t="shared" si="14"/>
         <v>9.1689473684210547</v>
       </c>
       <c r="F94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", E$24:E$80)</f>
+        <f t="shared" si="14"/>
         <v>17.158421052631578</v>
       </c>
       <c r="G94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", F$24:F$80)</f>
+        <f t="shared" si="14"/>
         <v>5.1336842105263161</v>
       </c>
       <c r="H94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", G$24:G$80)</f>
+        <f t="shared" si="14"/>
         <v>19.448421052631584</v>
       </c>
       <c r="I94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", H$24:H$80)</f>
+        <f t="shared" si="14"/>
         <v>36.605789473684204</v>
       </c>
       <c r="J94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", I$24:I$80)</f>
+        <f t="shared" si="14"/>
         <v>14.301052631578949</v>
       </c>
       <c r="K94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", J$24:J$80)</f>
+        <f t="shared" si="14"/>
         <v>181.55526315789476</v>
       </c>
       <c r="L94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", K$24:K$80)</f>
+        <f t="shared" si="14"/>
         <v>3.4178947368421051</v>
       </c>
       <c r="M94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", L$24:L$80)</f>
+        <f t="shared" si="14"/>
         <v>0.29894736842105263</v>
       </c>
       <c r="N94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", M$24:M$80)</f>
+        <f t="shared" si="14"/>
         <v>446.59700000000004</v>
       </c>
       <c r="O94" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "manual", N$24:N$80)</f>
+        <f t="shared" si="14"/>
         <v>134.35421052631574</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B95" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", B$24:B$80)</f>
+        <f t="shared" ref="C95:O95" si="15">AVERAGEIF($R$24:$R$80, "auto", B$24:B$80)</f>
         <v>4.5199999999999987</v>
       </c>
       <c r="D95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", C$24:C$80)</f>
+        <f t="shared" si="15"/>
         <v>79.543157894736837</v>
       </c>
       <c r="E95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", D$24:D$80)</f>
+        <f t="shared" si="15"/>
         <v>9.2989473684210537</v>
       </c>
       <c r="F95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", E$24:E$80)</f>
+        <f t="shared" si="15"/>
         <v>17.475789473684213</v>
       </c>
       <c r="G95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", F$24:F$80)</f>
+        <f t="shared" si="15"/>
         <v>5.2457894736842103</v>
       </c>
       <c r="H95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", G$24:G$80)</f>
+        <f t="shared" si="15"/>
         <v>19.844736842105267</v>
       </c>
       <c r="I95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", H$24:H$80)</f>
+        <f t="shared" si="15"/>
         <v>37.320526315789472</v>
       </c>
       <c r="J95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", I$24:I$80)</f>
+        <f t="shared" si="15"/>
         <v>14.544736842105261</v>
       </c>
       <c r="K95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", J$24:J$80)</f>
+        <f t="shared" si="15"/>
         <v>186.05368421052628</v>
       </c>
       <c r="L95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", K$24:K$80)</f>
+        <f t="shared" si="15"/>
         <v>3.5105263157894733</v>
       </c>
       <c r="M95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", L$24:L$80)</f>
+        <f t="shared" si="15"/>
         <v>0.29368421052631577</v>
       </c>
       <c r="N95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", M$24:M$80)</f>
+        <f t="shared" si="15"/>
         <v>236.57857142857142</v>
       </c>
       <c r="O95" s="29">
-        <f>AVERAGEIF($R$24:$R$80, "auto", N$24:N$80)</f>
+        <f t="shared" si="15"/>
         <v>140.43789473684208</v>
       </c>
     </row>
@@ -7404,7 +7404,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A98" s="26" t="s">
-        <v>104</v>
+        <v>165</v>
       </c>
       <c r="B98" s="32"/>
       <c r="C98" s="28"/>
@@ -7440,7 +7440,7 @@
     </row>
     <row r="100" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="B100" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C100" s="13" t="s">
         <v>92</v>
@@ -7485,128 +7485,128 @@
     <row r="101" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <f>COUNTIFS($R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="C101" s="29">
         <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>4.4455555555555542</v>
+        <v>3.8976923076923078</v>
       </c>
       <c r="D101" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>80.190555555555548</v>
+        <f t="shared" ref="C101:O101" si="16">AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
+        <v>80.826153846153844</v>
       </c>
       <c r="E101" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>8.7322222222222248</v>
+        <f t="shared" si="16"/>
+        <v>8.0299999999999994</v>
       </c>
       <c r="F101" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>15.93722222222222</v>
+        <f t="shared" si="16"/>
+        <v>14.919999999999998</v>
       </c>
       <c r="G101" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>5.007777777777779</v>
+        <f t="shared" si="16"/>
+        <v>4.5253846153846151</v>
       </c>
       <c r="H101" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>18.323333333333334</v>
+        <f t="shared" si="16"/>
+        <v>17.271538461538459</v>
       </c>
       <c r="I101" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>34.259444444444433</v>
+        <f t="shared" si="16"/>
+        <v>32.190000000000005</v>
       </c>
       <c r="J101" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>13.738333333333337</v>
+        <f t="shared" si="16"/>
+        <v>12.553076923076926</v>
       </c>
       <c r="K101" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>167.3705555555556</v>
+        <f t="shared" si="16"/>
+        <v>157.48076923076923</v>
       </c>
       <c r="L101" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>3.244444444444444</v>
+        <f t="shared" si="16"/>
+        <v>2.927692307692308</v>
       </c>
       <c r="M101" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>0.30722222222222217</v>
+        <f t="shared" si="16"/>
+        <v>0.28307692307692311</v>
       </c>
       <c r="N101" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>446.59700000000004</v>
+        <f t="shared" si="16"/>
+        <v>448.61222222222227</v>
       </c>
       <c r="O101" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "manual", $S$24:$S$80, "&lt;2")</f>
-        <v>113.28888888888892</v>
+        <f t="shared" si="16"/>
+        <v>111.50076923076927</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <f>COUNTIFS($R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C102" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>3.8039999999999998</v>
+        <f t="shared" ref="C102:O102" si="17">AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
+        <v>4.9369230769230761</v>
       </c>
       <c r="D102" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>82.285999999999987</v>
+        <f t="shared" si="17"/>
+        <v>78.513846153846146</v>
       </c>
       <c r="E102" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>6.7560000000000002</v>
+        <f t="shared" si="17"/>
+        <v>9.9769230769230752</v>
       </c>
       <c r="F102" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>11.491</v>
+        <f t="shared" si="17"/>
+        <v>18.519230769230766</v>
       </c>
       <c r="G102" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>4.2780000000000005</v>
+        <f t="shared" si="17"/>
+        <v>5.5623076923076926</v>
       </c>
       <c r="H102" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>14.475</v>
+        <f t="shared" si="17"/>
+        <v>21.134615384615383</v>
       </c>
       <c r="I102" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>25.964999999999996</v>
+        <f t="shared" si="17"/>
+        <v>39.653846153846153</v>
       </c>
       <c r="J102" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>11.035</v>
+        <f t="shared" si="17"/>
+        <v>15.538461538461535</v>
       </c>
       <c r="K102" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>119.78000000000002</v>
+        <f t="shared" si="17"/>
+        <v>199.29538461538456</v>
       </c>
       <c r="L102" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>2.5160000000000005</v>
+        <f t="shared" si="17"/>
+        <v>3.6276923076923073</v>
       </c>
       <c r="M102" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>0.26399999999999996</v>
+        <f t="shared" si="17"/>
+        <v>0.32615384615384618</v>
       </c>
       <c r="N102" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>222.72799999999998</v>
+        <f t="shared" si="17"/>
+        <v>313.44799999999998</v>
       </c>
       <c r="O102" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "auto", $S$24:$S$80, "&lt;2")</f>
-        <v>47.370000000000005</v>
+        <f t="shared" si="17"/>
+        <v>148.89923076923077</v>
       </c>
     </row>
     <row r="104" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="B104" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C104" s="13" t="s">
         <v>92</v>
@@ -7651,123 +7651,123 @@
     <row r="105" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <f>COUNTIFS($R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="C105" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>5.42</v>
+        <f t="shared" ref="C105:O105" si="18">AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
+        <v>5.794999999999999</v>
       </c>
       <c r="D105" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>69.06</v>
+        <f t="shared" si="18"/>
+        <v>76.958333333333329</v>
       </c>
       <c r="E105" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>17.03</v>
+        <f t="shared" si="18"/>
+        <v>11.636666666666668</v>
       </c>
       <c r="F105" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>39.14</v>
+        <f t="shared" si="18"/>
+        <v>22.008333333333336</v>
       </c>
       <c r="G105" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>7.4</v>
+        <f t="shared" si="18"/>
+        <v>6.4516666666666671</v>
       </c>
       <c r="H105" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>39.700000000000003</v>
+        <f t="shared" si="18"/>
+        <v>24.164999999999996</v>
       </c>
       <c r="I105" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>78.84</v>
+        <f t="shared" si="18"/>
+        <v>46.173333333333325</v>
       </c>
       <c r="J105" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>24.43</v>
+        <f t="shared" si="18"/>
+        <v>18.088333333333331</v>
       </c>
       <c r="K105" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>436.88</v>
+        <f t="shared" si="18"/>
+        <v>233.71666666666667</v>
       </c>
       <c r="L105" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>6.54</v>
+        <f t="shared" si="18"/>
+        <v>4.4800000000000004</v>
       </c>
       <c r="M105" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>0.15</v>
-      </c>
-      <c r="N105" s="29" t="e">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="18"/>
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="N105" s="29">
+        <f t="shared" si="18"/>
+        <v>428.46</v>
       </c>
       <c r="O105" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "manual", $S$24:$S$80, "&gt;1")</f>
-        <v>513.53</v>
+        <f t="shared" si="18"/>
+        <v>183.87</v>
       </c>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <f>COUNTIFS($R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C106" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>5.3155555555555551</v>
+        <f t="shared" ref="C106:O106" si="19">AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
+        <v>3.6166666666666667</v>
       </c>
       <c r="D106" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>76.495555555555555</v>
+        <f t="shared" si="19"/>
+        <v>81.773333333333341</v>
       </c>
       <c r="E106" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>12.124444444444443</v>
+        <f t="shared" si="19"/>
+        <v>7.830000000000001</v>
       </c>
       <c r="F106" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>24.125555555555554</v>
+        <f t="shared" si="19"/>
+        <v>15.214999999999998</v>
       </c>
       <c r="G106" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>6.3211111111111116</v>
+        <f t="shared" si="19"/>
+        <v>4.5599999999999996</v>
       </c>
       <c r="H106" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>25.811111111111117</v>
+        <f t="shared" si="19"/>
+        <v>17.049999999999997</v>
       </c>
       <c r="I106" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>49.937777777777782</v>
+        <f t="shared" si="19"/>
+        <v>32.265000000000008</v>
       </c>
       <c r="J106" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>18.444444444444443</v>
+        <f t="shared" si="19"/>
+        <v>12.391666666666666</v>
       </c>
       <c r="K106" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>259.69111111111107</v>
+        <f t="shared" si="19"/>
+        <v>157.36333333333334</v>
       </c>
       <c r="L106" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>4.615555555555555</v>
+        <f t="shared" si="19"/>
+        <v>3.2566666666666664</v>
       </c>
       <c r="M106" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>0.32666666666666672</v>
+        <f t="shared" si="19"/>
+        <v>0.22333333333333336</v>
       </c>
       <c r="N106" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>271.20500000000004</v>
+        <f t="shared" si="19"/>
+        <v>44.405000000000001</v>
       </c>
       <c r="O106" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "auto", $S$24:$S$80, "&gt;1")</f>
-        <v>243.84666666666666</v>
+        <f t="shared" si="19"/>
+        <v>122.10499999999998</v>
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.35">
@@ -7802,7 +7802,7 @@
     </row>
     <row r="109" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="B109" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>92</v>
@@ -7846,129 +7846,129 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
-        <f>COUNTIFS($R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>18</v>
+        <f>COUNTIFS($R$24:$R$80, "manual", $X$24:$X$80, "&lt;2")</f>
+        <v>11</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C110" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>4.4455555555555542</v>
+        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $X$24:$X$80, "&lt;2")</f>
+        <v>4.0609090909090915</v>
       </c>
       <c r="D110" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>80.190555555555548</v>
+        <f t="shared" ref="D110:O110" si="20">AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $X$24:$X$80, "&lt;2")</f>
+        <v>79.443636363636372</v>
       </c>
       <c r="E110" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>8.7322222222222248</v>
+        <f t="shared" si="20"/>
+        <v>8.7236363636363645</v>
       </c>
       <c r="F110" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>15.93722222222222</v>
+        <f t="shared" si="20"/>
+        <v>16.438181818181818</v>
       </c>
       <c r="G110" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>5.007777777777779</v>
+        <f t="shared" si="20"/>
+        <v>4.8672727272727272</v>
       </c>
       <c r="H110" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>18.323333333333334</v>
+        <f t="shared" si="20"/>
+        <v>18.658181818181816</v>
       </c>
       <c r="I110" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>34.259444444444433</v>
+        <f t="shared" si="20"/>
+        <v>35.094545454545454</v>
       </c>
       <c r="J110" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>13.738333333333337</v>
+        <f t="shared" si="20"/>
+        <v>13.589090909090912</v>
       </c>
       <c r="K110" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>167.3705555555556</v>
+        <f t="shared" si="20"/>
+        <v>173.39545454545453</v>
       </c>
       <c r="L110" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>3.244444444444444</v>
+        <f t="shared" si="20"/>
+        <v>3.1481818181818184</v>
       </c>
       <c r="M110" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>0.30722222222222217</v>
+        <f t="shared" si="20"/>
+        <v>0.29272727272727272</v>
       </c>
       <c r="N110" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>446.59700000000004</v>
+        <f t="shared" si="20"/>
+        <v>445.83714285714285</v>
       </c>
       <c r="O110" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "manual", $V$24:$V$80, "&lt;2")</f>
-        <v>113.28888888888892</v>
+        <f t="shared" si="20"/>
+        <v>127.1436363636364</v>
       </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
-        <f>COUNTIFS($R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>9</v>
+        <f>COUNTIFS($R$24:$R$80, "auto", $X$24:$X$80, "&lt;2")</f>
+        <v>5</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C111" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>3.6555555555555554</v>
+        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $X$24:$X$80, "&lt;2")</f>
+        <v>7.3439999999999994</v>
       </c>
       <c r="D111" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>82.952222222222218</v>
+        <f t="shared" ref="D111:O111" si="21">AVERAGEIFS(C$24:C$80, $R$24:$R$80, "auto", $X$24:$X$80, "&lt;2")</f>
+        <v>73.412000000000006</v>
       </c>
       <c r="E111" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>6.4911111111111115</v>
+        <f t="shared" si="21"/>
+        <v>14.357999999999999</v>
       </c>
       <c r="F111" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>11.037777777777778</v>
+        <f t="shared" si="21"/>
+        <v>27.921999999999997</v>
       </c>
       <c r="G111" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>4.0711111111111116</v>
+        <f t="shared" si="21"/>
+        <v>7.3459999999999992</v>
       </c>
       <c r="H111" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>13.606666666666667</v>
+        <f t="shared" si="21"/>
+        <v>32.832000000000008</v>
       </c>
       <c r="I111" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>24.643333333333331</v>
+        <f t="shared" si="21"/>
+        <v>60.758000000000003</v>
       </c>
       <c r="J111" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>10.562222222222223</v>
+        <f t="shared" si="21"/>
+        <v>21.704000000000001</v>
       </c>
       <c r="K111" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>113.95444444444446</v>
+        <f t="shared" si="21"/>
+        <v>337.34399999999999</v>
       </c>
       <c r="L111" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>2.3511111111111114</v>
+        <f t="shared" si="21"/>
+        <v>5.3759999999999994</v>
       </c>
       <c r="M111" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>0.24444444444444441</v>
-      </c>
-      <c r="N111" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>222.72799999999998</v>
+        <f t="shared" si="21"/>
+        <v>0.27</v>
+      </c>
+      <c r="N111" s="29" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="O111" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "auto", $V$24:$V$80, "&lt;2")</f>
-        <v>43.851111111111116</v>
+        <f t="shared" si="21"/>
+        <v>328.52599999999995</v>
       </c>
     </row>
     <row r="113" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="B113" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>92</v>
@@ -8012,124 +8012,124 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
-        <f>COUNTIFS($R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>1</v>
+        <f>COUNTIFS($R$24:$R$80, "manual", $X$24:$X$80, "&gt;1")</f>
+        <v>8</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C114" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>5.42</v>
+        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "manual", $X$24:$X$80, "&gt;1")</f>
+        <v>5.0962500000000004</v>
       </c>
       <c r="D114" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>69.06</v>
+        <f t="shared" ref="D114:O114" si="22">AVERAGEIFS(C$24:C$80, $R$24:$R$80, "manual", $X$24:$X$80, "&gt;1")</f>
+        <v>79.826250000000002</v>
       </c>
       <c r="E114" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>17.03</v>
+        <f t="shared" si="22"/>
+        <v>9.78125</v>
       </c>
       <c r="F114" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>39.14</v>
+        <f t="shared" si="22"/>
+        <v>18.14875</v>
       </c>
       <c r="G114" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>7.4</v>
+        <f t="shared" si="22"/>
+        <v>5.5</v>
       </c>
       <c r="H114" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>39.700000000000003</v>
+        <f t="shared" si="22"/>
+        <v>20.534999999999997</v>
       </c>
       <c r="I114" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>78.84</v>
+        <f t="shared" si="22"/>
+        <v>38.683749999999996</v>
       </c>
       <c r="J114" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>24.43</v>
+        <f t="shared" si="22"/>
+        <v>15.279999999999998</v>
       </c>
       <c r="K114" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>436.88</v>
+        <f t="shared" si="22"/>
+        <v>192.77500000000001</v>
       </c>
       <c r="L114" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>6.54</v>
+        <f t="shared" si="22"/>
+        <v>3.7887500000000003</v>
       </c>
       <c r="M114" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>0.15</v>
-      </c>
-      <c r="N114" s="29" t="e">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="22"/>
+        <v>0.30750000000000005</v>
+      </c>
+      <c r="N114" s="29">
+        <f t="shared" si="22"/>
+        <v>448.36999999999995</v>
       </c>
       <c r="O114" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "manual", $V$24:$V$80, "&gt;1")</f>
-        <v>513.53</v>
+        <f t="shared" si="22"/>
+        <v>144.26875000000001</v>
       </c>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
-        <f>COUNTIFS($R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>10</v>
+        <f>COUNTIFS($R$24:$R$80, "auto", $X$24:$X$80, "&gt;1")</f>
+        <v>14</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C115" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>5.298</v>
+        <f>AVERAGEIFS(B$24:B$80, $R$24:$R$80, "auto", $X$24:$X$80, "&gt;1")</f>
+        <v>3.5114285714285716</v>
       </c>
       <c r="D115" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>76.474999999999994</v>
+        <f t="shared" ref="D115:O115" si="23">AVERAGEIFS(C$24:C$80, $R$24:$R$80, "auto", $X$24:$X$80, "&gt;1")</f>
+        <v>81.732857142857142</v>
       </c>
       <c r="E115" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>11.825999999999999</v>
+        <f t="shared" si="23"/>
+        <v>7.4921428571428574</v>
       </c>
       <c r="F115" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>23.27</v>
+        <f t="shared" si="23"/>
+        <v>13.744999999999996</v>
       </c>
       <c r="G115" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>6.3029999999999999</v>
+        <f t="shared" si="23"/>
+        <v>4.4957142857142864</v>
       </c>
       <c r="H115" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>25.459000000000003</v>
+        <f t="shared" si="23"/>
+        <v>15.206428571428573</v>
       </c>
       <c r="I115" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>48.730000000000004</v>
+        <f t="shared" si="23"/>
+        <v>28.950000000000006</v>
       </c>
       <c r="J115" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>18.128999999999998</v>
+        <f t="shared" si="23"/>
+        <v>11.987857142857143</v>
       </c>
       <c r="K115" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>250.94299999999998</v>
+        <f t="shared" si="23"/>
+        <v>132.02142857142857</v>
       </c>
       <c r="L115" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>4.5539999999999994</v>
+        <f t="shared" si="23"/>
+        <v>2.8442857142857143</v>
       </c>
       <c r="M115" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>0.33800000000000002</v>
+        <f t="shared" si="23"/>
+        <v>0.30214285714285716</v>
       </c>
       <c r="N115" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>271.20500000000004</v>
+        <f t="shared" si="23"/>
+        <v>236.57857142857142</v>
       </c>
       <c r="O115" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $R$24:$R$80, "auto", $V$24:$V$80, "&gt;1")</f>
-        <v>227.36599999999999</v>
+        <f t="shared" si="23"/>
+        <v>73.26357142857141</v>
       </c>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.35">
@@ -8200,10 +8200,10 @@
     </row>
     <row r="120" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A120" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C120" s="13" t="s">
         <v>92</v>
@@ -8251,58 +8251,58 @@
         <v>5</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", B$24:B$80)</f>
+        <f t="shared" ref="C121:O121" si="24">AVERAGEIF($A$24:$A$80, "angelix*manual", B$24:B$80)</f>
         <v>6.4539999999999988</v>
       </c>
       <c r="D121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", C$24:C$80)</f>
+        <f t="shared" si="24"/>
         <v>72.91</v>
       </c>
       <c r="E121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", D$24:D$80)</f>
+        <f t="shared" si="24"/>
         <v>13.334</v>
       </c>
       <c r="F121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", E$24:E$80)</f>
+        <f t="shared" si="24"/>
         <v>25.648000000000003</v>
       </c>
       <c r="G121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", F$24:F$80)</f>
+        <f t="shared" si="24"/>
         <v>6.9539999999999988</v>
       </c>
       <c r="H121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", G$24:G$80)</f>
+        <f t="shared" si="24"/>
         <v>30.229999999999997</v>
       </c>
       <c r="I121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", H$24:H$80)</f>
+        <f t="shared" si="24"/>
         <v>55.878</v>
       </c>
       <c r="J121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", I$24:I$80)</f>
+        <f t="shared" si="24"/>
         <v>20.288</v>
       </c>
       <c r="K121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", J$24:J$80)</f>
+        <f t="shared" si="24"/>
         <v>295.21600000000001</v>
       </c>
       <c r="L121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", K$24:K$80)</f>
+        <f t="shared" si="24"/>
         <v>4.7520000000000007</v>
       </c>
       <c r="M121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", L$24:L$80)</f>
+        <f t="shared" si="24"/>
         <v>0.29599999999999999</v>
       </c>
       <c r="N121" s="29" t="e">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", M$24:M$80)</f>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O121" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*manual", N$24:N$80)</f>
+        <f t="shared" si="24"/>
         <v>244.15600000000001</v>
       </c>
     </row>
@@ -8312,58 +8312,58 @@
         <v>5</v>
       </c>
       <c r="B122" s="33" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", B$24:B$80)</f>
+        <f t="shared" ref="C122:O122" si="25">AVERAGEIF($A$24:$A$80, "angelix*auto", B$24:B$80)</f>
         <v>6.4539999999999988</v>
       </c>
       <c r="D122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", C$24:C$80)</f>
+        <f t="shared" si="25"/>
         <v>72.91</v>
       </c>
       <c r="E122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", D$24:D$80)</f>
+        <f t="shared" si="25"/>
         <v>13.367999999999999</v>
       </c>
       <c r="F122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", E$24:E$80)</f>
+        <f t="shared" si="25"/>
         <v>25.707999999999998</v>
       </c>
       <c r="G122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", F$24:F$80)</f>
+        <f t="shared" si="25"/>
         <v>6.9819999999999993</v>
       </c>
       <c r="H122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", G$24:G$80)</f>
+        <f t="shared" si="25"/>
         <v>30.318000000000001</v>
       </c>
       <c r="I122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", H$24:H$80)</f>
+        <f t="shared" si="25"/>
         <v>56.029999999999994</v>
       </c>
       <c r="J122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", I$24:I$80)</f>
+        <f t="shared" si="25"/>
         <v>20.350000000000001</v>
       </c>
       <c r="K122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", J$24:J$80)</f>
+        <f t="shared" si="25"/>
         <v>296.52600000000001</v>
       </c>
       <c r="L122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", K$24:K$80)</f>
+        <f t="shared" si="25"/>
         <v>4.8100000000000005</v>
       </c>
       <c r="M122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", L$24:L$80)</f>
+        <f t="shared" si="25"/>
         <v>0.29599999999999999</v>
       </c>
       <c r="N122" s="34" t="e">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", M$24:M$80)</f>
+        <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O122" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "angelix*auto", N$24:N$80)</f>
+        <f t="shared" si="25"/>
         <v>252.86999999999998</v>
       </c>
     </row>
@@ -8373,58 +8373,58 @@
         <v>12</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", B$24:B$80)</f>
+        <f t="shared" ref="C123:O123" si="26">AVERAGEIF($A$24:$A$80, "prophet*manual", B$24:B$80)</f>
         <v>3.2774999999999999</v>
       </c>
       <c r="D123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", C$24:C$80)</f>
+        <f t="shared" si="26"/>
         <v>83.060833333333321</v>
       </c>
       <c r="E123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", D$24:D$80)</f>
+        <f t="shared" si="26"/>
         <v>6.7716666666666683</v>
       </c>
       <c r="F123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", E$24:E$80)</f>
+        <f t="shared" si="26"/>
         <v>12.272500000000001</v>
       </c>
       <c r="G123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", F$24:F$80)</f>
+        <f t="shared" si="26"/>
         <v>4.046666666666666</v>
       </c>
       <c r="H123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", G$24:G$80)</f>
+        <f t="shared" si="26"/>
         <v>13.409999999999998</v>
       </c>
       <c r="I123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", H$24:H$80)</f>
+        <f t="shared" si="26"/>
         <v>25.680833333333329</v>
       </c>
       <c r="J123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", I$24:I$80)</f>
+        <f t="shared" si="26"/>
         <v>10.815833333333332</v>
       </c>
       <c r="K123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", J$24:J$80)</f>
+        <f t="shared" si="26"/>
         <v>116.72083333333335</v>
       </c>
       <c r="L123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", K$24:K$80)</f>
+        <f t="shared" si="26"/>
         <v>2.5791666666666671</v>
       </c>
       <c r="M123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", L$24:L$80)</f>
+        <f t="shared" si="26"/>
         <v>0.3</v>
       </c>
       <c r="N123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", M$24:M$80)</f>
+        <f t="shared" si="26"/>
         <v>446.59700000000004</v>
       </c>
       <c r="O123" s="29">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*manual", N$24:N$80)</f>
+        <f t="shared" si="26"/>
         <v>68.569999999999979</v>
       </c>
     </row>
@@ -8434,67 +8434,67 @@
         <v>12</v>
       </c>
       <c r="B124" s="33" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", B$24:B$80)</f>
+        <f t="shared" ref="C124:O124" si="27">AVERAGEIF($A$24:$A$80, "prophet*auto", B$24:B$80)</f>
         <v>3.3008333333333333</v>
       </c>
       <c r="D124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", C$24:C$80)</f>
+        <f t="shared" si="27"/>
         <v>82.963333333333324</v>
       </c>
       <c r="E124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", D$24:D$80)</f>
+        <f t="shared" si="27"/>
         <v>6.9375</v>
       </c>
       <c r="F124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", E$24:E$80)</f>
+        <f t="shared" si="27"/>
         <v>12.710833333333335</v>
       </c>
       <c r="G124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", F$24:F$80)</f>
+        <f t="shared" si="27"/>
         <v>4.2125000000000004</v>
       </c>
       <c r="H124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", G$24:G$80)</f>
+        <f t="shared" si="27"/>
         <v>13.925833333333335</v>
       </c>
       <c r="I124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", H$24:H$80)</f>
+        <f t="shared" si="27"/>
         <v>26.635833333333334</v>
       </c>
       <c r="J124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", I$24:I$80)</f>
+        <f t="shared" si="27"/>
         <v>11.15</v>
       </c>
       <c r="K124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", J$24:J$80)</f>
+        <f t="shared" si="27"/>
         <v>122.42333333333333</v>
       </c>
       <c r="L124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", K$24:K$80)</f>
+        <f t="shared" si="27"/>
         <v>2.7016666666666667</v>
       </c>
       <c r="M124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", L$24:L$80)</f>
+        <f t="shared" si="27"/>
         <v>0.29166666666666669</v>
       </c>
       <c r="N124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", M$24:M$80)</f>
+        <f t="shared" si="27"/>
         <v>236.57857142857142</v>
       </c>
       <c r="O124" s="34">
-        <f>AVERAGEIF($A$24:$A$80, "prophet*auto", N$24:N$80)</f>
+        <f t="shared" si="27"/>
         <v>73.433333333333323</v>
       </c>
     </row>
     <row r="127" spans="1:15" ht="28.8" x14ac:dyDescent="0.35">
       <c r="A127" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>92</v>
@@ -8542,58 +8542,58 @@
         <v>6</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C128" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" ref="C128:O128" si="28">AVERAGEIFS(B$24:B$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
         <v>6.9733333333333336</v>
       </c>
       <c r="D128" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>72.806666666666672</v>
       </c>
       <c r="E128" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>13.635</v>
       </c>
       <c r="F128" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>26.183333333333334</v>
       </c>
       <c r="G128" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>7.2716666666666656</v>
       </c>
       <c r="H128" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>31.47666666666667</v>
       </c>
       <c r="I128" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>57.66</v>
       </c>
       <c r="J128" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>20.906666666666666</v>
       </c>
       <c r="K128" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>311.64833333333331</v>
       </c>
       <c r="L128" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>5.0550000000000006</v>
       </c>
       <c r="M128" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>0.28499999999999998</v>
       </c>
       <c r="N128" s="29" t="e">
-        <f>AVERAGEIFS(M$24:M$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O128" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="28"/>
         <v>278.11499999999995</v>
       </c>
     </row>
@@ -8603,58 +8603,58 @@
         <v>6</v>
       </c>
       <c r="B129" s="33" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C129" s="34">
-        <f>AVERAGEIFS(B$24:B$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" ref="C129:O129" si="29">AVERAGEIFS(B$24:B$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
         <v>6.996666666666667</v>
       </c>
       <c r="D129" s="34">
-        <f>AVERAGEIFS(C$24:C$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>72.806666666666672</v>
       </c>
       <c r="E129" s="34">
-        <f>AVERAGEIFS(D$24:D$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>13.711666666666666</v>
       </c>
       <c r="F129" s="34">
-        <f>AVERAGEIFS(E$24:E$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>26.304999999999996</v>
       </c>
       <c r="G129" s="34">
-        <f>AVERAGEIFS(F$24:F$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>7.294999999999999</v>
       </c>
       <c r="H129" s="34">
-        <f>AVERAGEIFS(G$24:G$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>31.693333333333339</v>
       </c>
       <c r="I129" s="34">
-        <f>AVERAGEIFS(H$24:H$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>58.001666666666672</v>
       </c>
       <c r="J129" s="34">
-        <f>AVERAGEIFS(I$24:I$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>21.006666666666664</v>
       </c>
       <c r="K129" s="34">
-        <f>AVERAGEIFS(J$24:J$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>314.39</v>
       </c>
       <c r="L129" s="34">
-        <f>AVERAGEIFS(K$24:K$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>5.1033333333333335</v>
       </c>
       <c r="M129" s="34">
-        <f>AVERAGEIFS(L$24:L$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>0.28499999999999998</v>
       </c>
       <c r="N129" s="34" t="e">
-        <f>AVERAGEIFS(M$24:M$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O129" s="34">
-        <f>AVERAGEIFS(N$24:N$80, $P$24:$P$80, "True Semantic", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="29"/>
         <v>287.57666666666665</v>
       </c>
     </row>
@@ -8664,58 +8664,58 @@
         <v>13</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C130" s="29">
-        <f>AVERAGEIFS(B$24:B$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" ref="C130:O130" si="30">AVERAGEIFS(B$24:B$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
         <v>3.3538461538461539</v>
       </c>
       <c r="D130" s="29">
-        <f>AVERAGEIFS(C$24:C$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>82.742307692307705</v>
       </c>
       <c r="E130" s="29">
-        <f>AVERAGEIFS(D$24:D$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>7.1076923076923082</v>
       </c>
       <c r="F130" s="29">
-        <f>AVERAGEIFS(E$24:E$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>12.993076923076924</v>
       </c>
       <c r="G130" s="29">
-        <f>AVERAGEIFS(F$24:F$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>4.1469230769230769</v>
       </c>
       <c r="H130" s="29">
-        <f>AVERAGEIFS(G$24:G$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>13.896923076923077</v>
       </c>
       <c r="I130" s="29">
-        <f>AVERAGEIFS(H$24:H$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>26.888461538461534</v>
       </c>
       <c r="J130" s="29">
-        <f>AVERAGEIFS(I$24:I$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>11.252307692307692</v>
       </c>
       <c r="K130" s="29">
-        <f>AVERAGEIFS(J$24:J$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>121.5123076923077</v>
       </c>
       <c r="L130" s="29">
-        <f>AVERAGEIFS(K$24:K$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>2.6623076923076923</v>
       </c>
       <c r="M130" s="29">
-        <f>AVERAGEIFS(L$24:L$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>0.30538461538461542</v>
       </c>
       <c r="N130" s="29">
-        <f>AVERAGEIFS(M$24:M$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>446.59700000000004</v>
       </c>
       <c r="O130" s="29">
-        <f>AVERAGEIFS(N$24:N$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "manual")</f>
+        <f t="shared" si="30"/>
         <v>68.003076923076918</v>
       </c>
     </row>
@@ -8725,58 +8725,58 @@
         <v>13</v>
       </c>
       <c r="B131" s="33" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C131" s="34">
-        <f>AVERAGEIFS(B$24:B$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" ref="C131:O131" si="31">AVERAGEIFS(B$24:B$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
         <v>3.3769230769230774</v>
       </c>
       <c r="D131" s="34">
-        <f>AVERAGEIFS(C$24:C$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>82.652307692307687</v>
       </c>
       <c r="E131" s="34">
-        <f>AVERAGEIFS(D$24:D$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>7.2623076923076919</v>
       </c>
       <c r="F131" s="34">
-        <f>AVERAGEIFS(E$24:E$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>13.40076923076923</v>
       </c>
       <c r="G131" s="34">
-        <f>AVERAGEIFS(F$24:F$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>4.3000000000000007</v>
       </c>
       <c r="H131" s="34">
-        <f>AVERAGEIFS(G$24:G$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>14.376153846153848</v>
       </c>
       <c r="I131" s="34">
-        <f>AVERAGEIFS(H$24:H$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>27.775384615384613</v>
       </c>
       <c r="J131" s="34">
-        <f>AVERAGEIFS(I$24:I$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>11.562307692307693</v>
       </c>
       <c r="K131" s="34">
-        <f>AVERAGEIFS(J$24:J$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>126.82153846153847</v>
       </c>
       <c r="L131" s="34">
-        <f>AVERAGEIFS(K$24:K$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>2.7753846153846151</v>
       </c>
       <c r="M131" s="34">
-        <f>AVERAGEIFS(L$24:L$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>0.2976923076923077</v>
       </c>
       <c r="N131" s="34">
-        <f>AVERAGEIFS(M$24:M$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>236.57857142857142</v>
       </c>
       <c r="O131" s="34">
-        <f>AVERAGEIFS(N$24:N$80, $P$24:$P$80, "Machine Learning", $R$24:$R$80, "auto")</f>
+        <f t="shared" si="31"/>
         <v>72.527692307692305</v>
       </c>
     </row>
@@ -8784,7 +8784,7 @@
   <sortState ref="A27:R141">
     <sortCondition ref="R141"/>
   </sortState>
-  <conditionalFormatting sqref="C94:O94 C101:O101 C105:O105 C110:O110 C114:O114 C121:O121 C123:O123">
+  <conditionalFormatting sqref="C94:O94 C101:O101 C105:O105 C121:O121 C123:O123 C110:O110 C114:O114">
     <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>C95</formula>
     </cfRule>
@@ -8792,7 +8792,7 @@
       <formula>C95</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C95:O95 C102:O102 C106:O106 C111:O111 C115:O115 C122:O122 C124:O124">
+  <conditionalFormatting sqref="C95:O95 C102:O102 C106:O106 C122:O122 C124:O124 C111:O111 C115:O115">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>C94</formula>
     </cfRule>

</xml_diff>